<commit_message>
situacioni i perfunduar pa regjister sudi
</commit_message>
<xml_diff>
--- a/3-Katet/regjistri/Katet.xlsx
+++ b/3-Katet/regjistri/Katet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Katet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="22">
   <si>
     <t>Nr.</t>
   </si>
@@ -56,44 +56,47 @@
     <t>Gjithsej:</t>
   </si>
   <si>
-    <t>Sipërfaqja</t>
-  </si>
-  <si>
-    <t>(m²)</t>
-  </si>
-  <si>
-    <t>Nenkulm</t>
-  </si>
-  <si>
     <t>Nënkulm</t>
   </si>
   <si>
     <t>GARAZHA</t>
   </si>
   <si>
-    <t>PERDHESE</t>
-  </si>
-  <si>
-    <t>SHKALLA</t>
-  </si>
-  <si>
-    <t>PERDHES-TERASË</t>
-  </si>
-  <si>
-    <t>PUSET-FEKALE</t>
-  </si>
-  <si>
-    <t>SHTYLLE-ELEKTRIKE</t>
+    <t>SHKALLËT</t>
+  </si>
+  <si>
+    <t>PËRDHESË-TERASË</t>
+  </si>
+  <si>
+    <t>PËRDHESË</t>
+  </si>
+  <si>
+    <t>PUSETË-FEKALE</t>
+  </si>
+  <si>
+    <t>Përdhesa</t>
+  </si>
+  <si>
+    <t>Shkallët</t>
+  </si>
+  <si>
+    <t>Garazha</t>
+  </si>
+  <si>
+    <t>NËNKULM</t>
+  </si>
+  <si>
+    <t>NËNKULM-TERASË</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,7 +134,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -154,11 +157,79 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -188,6 +259,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -249,7 +344,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -281,9 +376,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -315,6 +411,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -490,33 +587,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:K25"/>
+  <dimension ref="B1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13:I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="1"/>
-    <col min="9" max="9" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B1" s="4"/>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -528,7 +623,7 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="2:11">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
@@ -550,13 +645,13 @@
       <c r="H2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="10"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="2:11">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="5">
         <v>12</v>
       </c>
@@ -570,14 +665,22 @@
         <v>616.5</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-    </row>
-    <row r="4" spans="2:11">
+        <v>12</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="15">
+        <v>94.96</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="5">
         <v>13</v>
       </c>
@@ -591,14 +694,14 @@
         <v>616.56600000000003</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-    </row>
-    <row r="5" spans="2:11">
+        <v>15</v>
+      </c>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
         <v>15</v>
       </c>
@@ -612,14 +715,14 @@
         <v>616.5</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-    </row>
-    <row r="6" spans="2:11">
+        <v>15</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="5">
         <v>16</v>
       </c>
@@ -633,14 +736,14 @@
         <v>616.5</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-    </row>
-    <row r="7" spans="2:11">
+        <v>13</v>
+      </c>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="5">
         <v>17</v>
       </c>
@@ -654,14 +757,14 @@
         <v>616.50300000000004</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-    </row>
-    <row r="8" spans="2:11">
+        <v>13</v>
+      </c>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="5">
         <v>18</v>
       </c>
@@ -675,20 +778,20 @@
         <v>616.50599999999997</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="I8" s="11">
-        <v>61.7</v>
-      </c>
-      <c r="J8" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="15"/>
+      <c r="H8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="12">
+        <v>27.27</v>
+      </c>
+      <c r="J8" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:11">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <v>19</v>
       </c>
@@ -702,14 +805,14 @@
         <v>616.40700000000004</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-    </row>
-    <row r="10" spans="2:11">
+        <v>14</v>
+      </c>
+      <c r="G9" s="15"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>20</v>
       </c>
@@ -723,20 +826,14 @@
         <v>616.375</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" s="11">
-        <v>53.49</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11">
+        <v>14</v>
+      </c>
+      <c r="G10" s="15"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="5">
         <v>25</v>
       </c>
@@ -750,14 +847,20 @@
         <v>618.98800000000006</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-    </row>
-    <row r="12" spans="2:11">
+        <v>15</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="15">
+        <v>5.76</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
         <v>27</v>
       </c>
@@ -771,14 +874,14 @@
         <v>622.34799999999996</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-    </row>
-    <row r="13" spans="2:11">
+        <v>15</v>
+      </c>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="5">
         <v>52</v>
       </c>
@@ -792,14 +895,20 @@
         <v>616.77700000000004</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-    </row>
-    <row r="14" spans="2:11">
+        <v>16</v>
+      </c>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="15">
+        <v>10.46</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
         <v>53</v>
       </c>
@@ -813,14 +922,14 @@
         <v>616.73400000000004</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-    </row>
-    <row r="15" spans="2:11">
+        <v>16</v>
+      </c>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="5">
         <v>55</v>
       </c>
@@ -834,21 +943,21 @@
         <v>616.5</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="I15" s="11">
-        <f>SUM(I3:I10)</f>
-        <v>115.19</v>
-      </c>
-      <c r="J15" s="11" t="s">
+      <c r="I15" s="15">
+        <f>SUM(I3:I14)</f>
+        <v>138.44999999999999</v>
+      </c>
+      <c r="J15" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="2:11">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="5">
         <v>56</v>
       </c>
@@ -862,14 +971,14 @@
         <v>622.34799999999996</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-    </row>
-    <row r="17" spans="2:10">
+        <v>12</v>
+      </c>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="5">
         <v>57</v>
       </c>
@@ -883,175 +992,520 @@
         <v>622.34799999999996</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-    </row>
-    <row r="18" spans="2:10">
-      <c r="B18" s="5">
-        <v>58</v>
-      </c>
-      <c r="C18" s="6">
-        <v>7511886.2640000004</v>
-      </c>
-      <c r="D18" s="6">
-        <v>4692127.466</v>
-      </c>
-      <c r="E18" s="6">
-        <v>622.01</v>
-      </c>
-      <c r="F18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I20" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="J20" s="19"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="3">
+        <v>7</v>
+      </c>
+      <c r="C21" s="2">
+        <v>4692113.6940000001</v>
+      </c>
+      <c r="D21" s="2">
+        <v>7511885.301</v>
+      </c>
+      <c r="E21" s="2">
+        <v>619.59</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-    </row>
-    <row r="21" spans="2:10">
-      <c r="B21" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I21" s="8" t="s">
+      <c r="G21" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="J21" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10">
+      <c r="H21" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" s="15">
+        <v>100.46</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="C22" s="2">
-        <v>7512505.9000000004</v>
+        <v>4692123.8839999996</v>
       </c>
       <c r="D22" s="2">
-        <v>4692042.443</v>
+        <v>7511886.2280000001</v>
       </c>
       <c r="E22" s="2">
-        <v>633</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="I22" s="11">
-        <v>54.68</v>
-      </c>
-      <c r="J22" s="11" t="s">
+        <v>619.59</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="3">
+        <v>31</v>
+      </c>
+      <c r="C23" s="2">
+        <v>4692124.8080000002</v>
+      </c>
+      <c r="D23" s="2">
+        <v>7511876.3559999997</v>
+      </c>
+      <c r="E23" s="2">
+        <v>619.59</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="3">
+        <v>32</v>
+      </c>
+      <c r="C24" s="2">
+        <v>4692123.2970000003</v>
+      </c>
+      <c r="D24" s="2">
+        <v>7511876.2089999998</v>
+      </c>
+      <c r="E24" s="2">
+        <v>619.59</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="11">
+        <v>33</v>
+      </c>
+      <c r="C25" s="2">
+        <v>4692123.2389000002</v>
+      </c>
+      <c r="D25" s="2">
+        <v>7511876.8300000001</v>
+      </c>
+      <c r="E25" s="2">
+        <v>619.59</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="11">
+        <v>34</v>
+      </c>
+      <c r="C26" s="2">
+        <v>4692121.0130000003</v>
+      </c>
+      <c r="D26" s="2">
+        <v>7511876.6040000003</v>
+      </c>
+      <c r="E26" s="2">
+        <v>619.59</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="11">
+        <v>35</v>
+      </c>
+      <c r="C27" s="2">
+        <v>4692121.091</v>
+      </c>
+      <c r="D27" s="2">
+        <v>7511875.7060000002</v>
+      </c>
+      <c r="E27" s="2">
+        <v>619.59</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="11">
+        <v>36</v>
+      </c>
+      <c r="C28" s="2">
+        <v>4692120.2690000003</v>
+      </c>
+      <c r="D28" s="2">
+        <v>7511875.1720000003</v>
+      </c>
+      <c r="E28" s="2">
+        <v>619.59</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="11">
+        <v>37</v>
+      </c>
+      <c r="C29" s="2">
+        <v>4692119.3109999998</v>
+      </c>
+      <c r="D29" s="2">
+        <v>7511875.0939999996</v>
+      </c>
+      <c r="E29" s="2">
+        <v>619.59</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="11">
+        <v>38</v>
+      </c>
+      <c r="C30" s="2">
+        <v>4692118.3782000002</v>
+      </c>
+      <c r="D30" s="2">
+        <v>7511875.4614000004</v>
+      </c>
+      <c r="E30" s="2">
+        <v>619.59</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="11">
+        <v>39</v>
+      </c>
+      <c r="C31" s="2">
+        <v>4692118.2939999998</v>
+      </c>
+      <c r="D31" s="2">
+        <v>7511876.3606000002</v>
+      </c>
+      <c r="E31" s="2">
+        <v>619.59</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="11">
+        <v>41</v>
+      </c>
+      <c r="C32" s="2">
+        <v>4692116.0829999996</v>
+      </c>
+      <c r="D32" s="2">
+        <v>7511876.1749999998</v>
+      </c>
+      <c r="E32" s="2">
+        <v>619.59</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I32" s="15">
+        <v>1.67</v>
+      </c>
+      <c r="J32" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="2:10">
-      <c r="B23" s="3">
-        <v>3</v>
-      </c>
-      <c r="C23" s="2">
-        <v>7512510.1579999998</v>
-      </c>
-      <c r="D23" s="2">
-        <v>4692039.1689999998</v>
-      </c>
-      <c r="E23" s="2">
-        <v>633</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-    </row>
-    <row r="24" spans="2:10">
-      <c r="B24" s="3">
-        <v>4</v>
-      </c>
-      <c r="C24" s="2">
-        <v>7512516.3631999996</v>
-      </c>
-      <c r="D24" s="2">
-        <v>4692047.2391999997</v>
-      </c>
-      <c r="E24" s="2">
-        <v>633</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-    </row>
-    <row r="25" spans="2:10">
-      <c r="B25" s="3">
-        <v>5</v>
-      </c>
-      <c r="C25" s="2">
-        <v>7512512.1052000001</v>
-      </c>
-      <c r="D25" s="2">
-        <v>4692050.5131999999</v>
-      </c>
-      <c r="E25" s="2">
-        <v>633</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="11">
+        <v>42</v>
+      </c>
+      <c r="C33" s="2">
+        <v>4692116.1270000003</v>
+      </c>
+      <c r="D33" s="2">
+        <v>7511875.5580000002</v>
+      </c>
+      <c r="E33" s="2">
+        <v>619.59</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="11">
+        <v>43</v>
+      </c>
+      <c r="C34" s="2">
+        <v>4692114.6179999998</v>
+      </c>
+      <c r="D34" s="2">
+        <v>7511875.4289999995</v>
+      </c>
+      <c r="E34" s="2">
+        <v>619.59</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B35" s="11">
+        <v>44</v>
+      </c>
+      <c r="C35" s="2">
+        <v>4692116.1213999996</v>
+      </c>
+      <c r="D35" s="2">
+        <v>7511875.6360999998</v>
+      </c>
+      <c r="E35" s="2">
+        <v>619.59</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I35" s="15">
+        <v>1.67</v>
+      </c>
+      <c r="J35" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B36" s="11">
+        <v>45</v>
+      </c>
+      <c r="C36" s="2">
+        <v>4692117.2120000003</v>
+      </c>
+      <c r="D36" s="2">
+        <v>7511875.5</v>
+      </c>
+      <c r="E36" s="2">
+        <v>619.59</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B37" s="11">
+        <v>46</v>
+      </c>
+      <c r="C37" s="2">
+        <v>4692118.3735999996</v>
+      </c>
+      <c r="D37" s="2">
+        <v>7511875.5099999998</v>
+      </c>
+      <c r="E37" s="2">
+        <v>619.59</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B38" s="11">
+        <v>47</v>
+      </c>
+      <c r="C38" s="2">
+        <v>4692121.0855999999</v>
+      </c>
+      <c r="D38" s="2">
+        <v>7511875.7685000002</v>
+      </c>
+      <c r="E38" s="2">
+        <v>619.59</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G38" s="15"/>
+      <c r="H38" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I38" s="12">
+        <f>SUM(I21:I36)</f>
+        <v>103.8</v>
+      </c>
+      <c r="J38" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="11">
+        <v>48</v>
+      </c>
+      <c r="C39" s="2">
+        <v>4692121.8990000002</v>
+      </c>
+      <c r="D39" s="2">
+        <v>7511875.8830000004</v>
+      </c>
+      <c r="E39" s="2">
+        <v>619.59</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G39" s="15"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B40" s="11">
+        <v>49</v>
+      </c>
+      <c r="C40" s="2">
+        <v>4692123.2879999997</v>
+      </c>
+      <c r="D40" s="2">
+        <v>7511876.3048999999</v>
+      </c>
+      <c r="E40" s="2">
+        <v>619.59</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G40" s="15"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="G22:G25"/>
-    <mergeCell ref="H22:H25"/>
-    <mergeCell ref="I22:I25"/>
-    <mergeCell ref="J22:J25"/>
+  <mergeCells count="31">
     <mergeCell ref="I2:J2"/>
-    <mergeCell ref="G3:G18"/>
+    <mergeCell ref="G3:G17"/>
     <mergeCell ref="H3:H7"/>
     <mergeCell ref="I3:I7"/>
     <mergeCell ref="J3:J7"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="H10:H14"/>
-    <mergeCell ref="I10:I14"/>
-    <mergeCell ref="J10:J14"/>
-    <mergeCell ref="H15:H18"/>
-    <mergeCell ref="I15:I18"/>
-    <mergeCell ref="J15:J18"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="J8:J10"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="I32:I34"/>
+    <mergeCell ref="J32:J34"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="J38:J40"/>
+    <mergeCell ref="G21:G40"/>
+    <mergeCell ref="I38:I40"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="I35:I37"/>
+    <mergeCell ref="J35:J37"/>
+    <mergeCell ref="H21:H31"/>
+    <mergeCell ref="I21:I31"/>
+    <mergeCell ref="J21:J31"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
permirsim i katit nenkulm ne kati 1
</commit_message>
<xml_diff>
--- a/3-Katet/regjistri/Katet.xlsx
+++ b/3-Katet/regjistri/Katet.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="21">
   <si>
     <t>Nr.</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Gjithsej:</t>
   </si>
   <si>
-    <t>Nënkulm</t>
-  </si>
-  <si>
     <t>GARAZHA</t>
   </si>
   <si>
@@ -83,10 +80,10 @@
     <t>Garazha</t>
   </si>
   <si>
-    <t>NËNKULM</t>
-  </si>
-  <si>
-    <t>NËNKULM-TERASË</t>
+    <t>Kati1</t>
+  </si>
+  <si>
+    <t>Kati1-TERASË</t>
   </si>
 </sst>
 </file>
@@ -593,8 +590,8 @@
   </sheetPr>
   <dimension ref="B1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13:I14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,13 +662,13 @@
         <v>616.5</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I3" s="15">
         <v>94.96</v>
@@ -694,7 +691,7 @@
         <v>616.56600000000003</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
@@ -715,7 +712,7 @@
         <v>616.5</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
@@ -736,7 +733,7 @@
         <v>616.5</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
@@ -757,7 +754,7 @@
         <v>616.50300000000004</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
@@ -778,11 +775,11 @@
         <v>616.50599999999997</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G8" s="15"/>
       <c r="H8" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I8" s="12">
         <v>27.27</v>
@@ -805,7 +802,7 @@
         <v>616.40700000000004</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G9" s="15"/>
       <c r="H9" s="13"/>
@@ -826,7 +823,7 @@
         <v>616.375</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G10" s="15"/>
       <c r="H10" s="14"/>
@@ -847,11 +844,11 @@
         <v>618.98800000000006</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G11" s="15"/>
       <c r="H11" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I11" s="15">
         <v>5.76</v>
@@ -874,7 +871,7 @@
         <v>622.34799999999996</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
@@ -895,7 +892,7 @@
         <v>616.77700000000004</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G13" s="15"/>
       <c r="H13" s="15" t="s">
@@ -922,7 +919,7 @@
         <v>616.73400000000004</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
@@ -943,7 +940,7 @@
         <v>616.5</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G15" s="15"/>
       <c r="H15" s="15" t="s">
@@ -971,7 +968,7 @@
         <v>622.34799999999996</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
@@ -992,7 +989,7 @@
         <v>622.34799999999996</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
@@ -1040,13 +1037,13 @@
         <v>619.59</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="I21" s="15">
         <v>100.46</v>
@@ -1069,7 +1066,7 @@
         <v>619.59</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
@@ -1090,7 +1087,7 @@
         <v>619.59</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
@@ -1111,7 +1108,7 @@
         <v>619.59</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
@@ -1132,7 +1129,7 @@
         <v>619.59</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
@@ -1153,7 +1150,7 @@
         <v>619.59</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
@@ -1174,7 +1171,7 @@
         <v>619.59</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
@@ -1195,7 +1192,7 @@
         <v>619.59</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
@@ -1216,7 +1213,7 @@
         <v>619.59</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
@@ -1237,7 +1234,7 @@
         <v>619.59</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G30" s="15"/>
       <c r="H30" s="15"/>
@@ -1258,7 +1255,7 @@
         <v>619.59</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
@@ -1279,7 +1276,7 @@
         <v>619.59</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G32" s="15"/>
       <c r="H32" s="15" t="s">
@@ -1306,7 +1303,7 @@
         <v>619.59</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G33" s="15"/>
       <c r="H33" s="15"/>
@@ -1327,7 +1324,7 @@
         <v>619.59</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
@@ -1348,7 +1345,7 @@
         <v>619.59</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G35" s="15"/>
       <c r="H35" s="15" t="s">
@@ -1375,7 +1372,7 @@
         <v>619.59</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G36" s="15"/>
       <c r="H36" s="15"/>
@@ -1396,7 +1393,7 @@
         <v>619.59</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G37" s="15"/>
       <c r="H37" s="15"/>
@@ -1417,7 +1414,7 @@
         <v>619.59</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G38" s="15"/>
       <c r="H38" s="16" t="s">
@@ -1445,7 +1442,7 @@
         <v>619.59</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G39" s="15"/>
       <c r="H39" s="17"/>
@@ -1466,7 +1463,7 @@
         <v>619.59</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G40" s="15"/>
       <c r="H40" s="18"/>

</xml_diff>